<commit_message>
Added ESP tests tick chart
</commit_message>
<xml_diff>
--- a/04_Etude/Bilans de consommation.xlsx
+++ b/04_Etude/Bilans de consommation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandre.PICOTTE\Documents\P1704_Manettes\04_Etude\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\projet_manette\manette\04_Etude\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>Arduino Mega</t>
   </si>
@@ -60,28 +60,28 @@
     <t>Calcul</t>
   </si>
   <si>
-    <t>12h</t>
-  </si>
-  <si>
     <t>mAh</t>
   </si>
   <si>
-    <t>2600 mAh</t>
-  </si>
-  <si>
-    <t>2600/140.93*0.7</t>
-  </si>
-  <si>
     <t>2600/195.93*0.7</t>
   </si>
   <si>
     <t>9h</t>
+  </si>
+  <si>
+    <t>Autonomie de la manette</t>
+  </si>
+  <si>
+    <t>Rendement:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="hh\.mm&quot; h&quot;;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -143,6 +143,13 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,7 +471,7 @@
         <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -511,7 +518,7 @@
         <v>195.93</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -520,7 +527,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -535,93 +542,124 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E5" sqref="E5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>0.93</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>50</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>50</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="3">
-        <f>SUM(B:B)</f>
+      <c r="B6" s="3">
+        <f>SUM(B1:B5)</f>
         <v>140.93</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2600</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>9</v>
+    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="5" t="s">
-        <v>11</v>
+      <c r="C8" s="7">
+        <f>E6*A10/B6</f>
+        <v>12.914212729723975</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <f>70%</f>
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E5:F5"/>
+  </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>